<commit_message>
Updates for extended checking & better logging
This also checks out the main branch that is required for
validating changes.
</commit_message>
<xml_diff>
--- a/templates/voc4cat_template_043.xlsx
+++ b/templates/voc4cat_template_043.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-template\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-dalito\voc4cat-template\inbox-excel-vocabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5279714C-CB90-44D9-8E9A-A63F98EB4A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4713931-A8D2-48FF-BCB2-DE58DB339F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="15825" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="119">
   <si>
     <t>0.4.3</t>
   </si>
@@ -346,16 +346,10 @@
     <t>ex:c03</t>
   </si>
   <si>
-    <t>ex:col1</t>
-  </si>
-  <si>
     <t>Linked data term</t>
   </si>
   <si>
     <t>ex:c01, ex:c02, ex:c03</t>
-  </si>
-  <si>
-    <t>voc4cat-template</t>
   </si>
   <si>
     <t>Collection of term related to linked data.</t>
@@ -1574,6 +1568,12 @@
   </si>
   <si>
     <t>2023-06a</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-2345-6789 Sofia Garcia</t>
+  </si>
+  <si>
+    <t>ex:c10</t>
   </si>
 </sst>
 </file>
@@ -2469,8 +2469,8 @@
   </sheetPr>
   <dimension ref="A11:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2497,15 +2497,15 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -2660,7 +2660,7 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2728,7 +2728,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2741,10 +2741,10 @@
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>96</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
@@ -2754,10 +2754,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>95</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>97</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
@@ -2778,7 +2778,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -3153,7 +3153,7 @@
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
@@ -3607,7 +3607,7 @@
     <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B88" s="27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C88" s="27"/>
       <c r="D88" s="27"/>
@@ -3907,7 +3907,7 @@
     <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B116" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
@@ -4064,7 +4064,7 @@
     <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B131" s="27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
@@ -4188,7 +4188,7 @@
     <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B143" s="28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -4245,18 +4245,18 @@
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D148" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="149" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D149" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
@@ -5338,8 +5338,8 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5458,10 +5458,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>10</v>
@@ -5472,7 +5472,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>12</v>
@@ -5486,7 +5486,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>14</v>
@@ -6502,8 +6502,8 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6521,7 +6521,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6558,13 +6558,13 @@
         <v>66</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>67</v>
@@ -6575,17 +6575,19 @@
       <c r="G3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="9"/>
+      <c r="H3" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>67</v>
@@ -6600,10 +6602,12 @@
         <v>73</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -6625,10 +6629,12 @@
         <v>82</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="9"/>
+      <c r="H5" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
@@ -6638,7 +6644,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6797,7 +6803,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{6F1BA696-5625-486F-8DDA-D4DF87BC6835}"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{6F1BA696-5625-486F-8DDA-D4DF87BC6835}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
@@ -6816,7 +6822,7 @@
   <dimension ref="A1:F485"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7357,7 +7363,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7385,27 +7391,27 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>87</v>
+      <c r="E3" s="17" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -7581,7 +7587,7 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>